<commit_message>
Corrected reading in damages and added Wind layer turbine assumption to assumptions.xlsx file instead of config
</commit_message>
<xml_diff>
--- a/assumptions/assumptions.xlsx
+++ b/assumptions/assumptions.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Master_Thesis\WIPLEX\assumptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F8C7C3-54D0-40CF-99B3-746F7CD3F283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C90AF0-A025-4C8F-8C02-54F895171413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
-    <sheet name="Turbine_Types" sheetId="6" r:id="rId2"/>
-    <sheet name="Power_Coefficient" sheetId="7" r:id="rId3"/>
-    <sheet name="Sze1" sheetId="2" r:id="rId4"/>
-    <sheet name="Sze2" sheetId="3" r:id="rId5"/>
-    <sheet name="Sze3" sheetId="4" r:id="rId6"/>
-    <sheet name="Sze4" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
+    <sheet name="Turbine_Types" sheetId="6" r:id="rId3"/>
+    <sheet name="Power_Coefficient" sheetId="7" r:id="rId4"/>
+    <sheet name="Sze1" sheetId="2" r:id="rId5"/>
+    <sheet name="Sze2" sheetId="3" r:id="rId6"/>
+    <sheet name="Sze3" sheetId="4" r:id="rId7"/>
+    <sheet name="Sze4" sheetId="5" r:id="rId8"/>
+    <sheet name="Sze5" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="101">
   <si>
     <t>Lower</t>
   </si>
@@ -144,15 +146,6 @@
     <t>Grid connection (million €)</t>
   </si>
   <si>
-    <t>(50, 100)</t>
-  </si>
-  <si>
-    <t>(100, 150)</t>
-  </si>
-  <si>
-    <t>(150, 200)</t>
-  </si>
-  <si>
     <t>Wind Class</t>
   </si>
   <si>
@@ -162,9 +155,6 @@
     <t>iec3</t>
   </si>
   <si>
-    <t>Wind speed layer (m)</t>
-  </si>
-  <si>
     <t>Installation cost (€/kW)</t>
   </si>
   <si>
@@ -208,6 +198,153 @@
   </si>
   <si>
     <t>Power Coefficients</t>
+  </si>
+  <si>
+    <t>Wind layer (m)</t>
+  </si>
+  <si>
+    <t>New Turbines</t>
+  </si>
+  <si>
+    <t>E-141 EP4</t>
+  </si>
+  <si>
+    <t>129/159</t>
+  </si>
+  <si>
+    <t>IIIa</t>
+  </si>
+  <si>
+    <t>E-126 EP4</t>
+  </si>
+  <si>
+    <t>IIa</t>
+  </si>
+  <si>
+    <t>99/135/144</t>
+  </si>
+  <si>
+    <t>E-126 7.580</t>
+  </si>
+  <si>
+    <t>Ia</t>
+  </si>
+  <si>
+    <t>E-115 3.000</t>
+  </si>
+  <si>
+    <t>92/135/149</t>
+  </si>
+  <si>
+    <t>E-115 2.500</t>
+  </si>
+  <si>
+    <t>92.5/149</t>
+  </si>
+  <si>
+    <t>E-112/45.114</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/1297-enercon-e-141-ep4</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/1183-enercon-e-126-ep4</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/14-enercon-e-126-7.580</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/832-enercon-e-115-3.000</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/113-enercon-e-112-45.114</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/427-enercon-e-115-2.500</t>
+  </si>
+  <si>
+    <t>IEC S</t>
+  </si>
+  <si>
+    <t>E-101</t>
+  </si>
+  <si>
+    <t>99/124/135/149</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/130-enercon-e-101</t>
+  </si>
+  <si>
+    <t>E-101 E2 3.050</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/935-enercon-e-101-e2-3.050</t>
+  </si>
+  <si>
+    <t>E-92</t>
+  </si>
+  <si>
+    <t>78/84/85/98/104/108/138</t>
+  </si>
+  <si>
+    <t>E-82 E2 2.300</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/131-enercon-e-92</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/550-enercon-e-82-e2-2.300</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/835-enercon-e-82-e2-2.000</t>
+  </si>
+  <si>
+    <t>E-82 E2 2.000</t>
+  </si>
+  <si>
+    <t>78/85/98/108/138</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/1487-enercon-e-82-e4-2.350</t>
+  </si>
+  <si>
+    <t>E-82 E4 2.350</t>
+  </si>
+  <si>
+    <t>59/69/78/84</t>
+  </si>
+  <si>
+    <t>E-82 E4 3.000</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Currently Available</t>
+  </si>
+  <si>
+    <t>59/ 69/ 78/ 84</t>
+  </si>
+  <si>
+    <t>E-70 E4 2.300</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/833-enercon-e-82-e4-3.000</t>
+  </si>
+  <si>
+    <t>https://www.wind-turbine-models.com/turbines/69-enercon-e-70-e4-2.300</t>
+  </si>
+  <si>
+    <t>58/64/70/85/98/99/113</t>
+  </si>
+  <si>
+    <t>E-66/18.70</t>
+  </si>
+  <si>
+    <t>65/80/86/98/114</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -573,20 +710,20 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -597,7 +734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -608,7 +745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -619,7 +756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -630,7 +767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -647,37 +784,428 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E3D0C2-3B2F-418A-A4B6-454C361CDD1D}">
+  <dimension ref="A1:P20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" t="s">
+        <v>94</v>
+      </c>
+      <c r="P3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4">
+        <v>135</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4">
+        <v>124</v>
+      </c>
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4">
+        <v>74</v>
+      </c>
+      <c r="J4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O4" t="s">
+        <v>97</v>
+      </c>
+      <c r="P4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>141</v>
+      </c>
+      <c r="C5">
+        <v>127</v>
+      </c>
+      <c r="D5">
+        <v>127</v>
+      </c>
+      <c r="E5">
+        <v>115.7</v>
+      </c>
+      <c r="F5">
+        <v>115</v>
+      </c>
+      <c r="G5">
+        <v>114</v>
+      </c>
+      <c r="H5">
+        <v>101</v>
+      </c>
+      <c r="I5">
+        <v>101</v>
+      </c>
+      <c r="J5">
+        <v>92</v>
+      </c>
+      <c r="K5">
+        <v>82</v>
+      </c>
+      <c r="L5">
+        <v>82</v>
+      </c>
+      <c r="M5">
+        <v>82</v>
+      </c>
+      <c r="N5">
+        <v>82</v>
+      </c>
+      <c r="O5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>4.2</v>
+      </c>
+      <c r="C8">
+        <v>4.2</v>
+      </c>
+      <c r="D8">
+        <v>7.58</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>2.5</v>
+      </c>
+      <c r="G8">
+        <v>4.5</v>
+      </c>
+      <c r="H8">
+        <v>3.05</v>
+      </c>
+      <c r="I8">
+        <v>3.05</v>
+      </c>
+      <c r="J8">
+        <v>2.35</v>
+      </c>
+      <c r="K8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>2.35</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P8">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" t="s">
+        <v>61</v>
+      </c>
+      <c r="O18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K19" t="s">
+        <v>100</v>
+      </c>
+      <c r="L19" t="s">
+        <v>100</v>
+      </c>
+      <c r="M19" t="s">
+        <v>100</v>
+      </c>
+      <c r="N19" t="s">
+        <v>100</v>
+      </c>
+      <c r="O19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J20" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" t="s">
+        <v>83</v>
+      </c>
+      <c r="L20" t="s">
+        <v>84</v>
+      </c>
+      <c r="M20" t="s">
+        <v>87</v>
+      </c>
+      <c r="N20" t="s">
+        <v>95</v>
+      </c>
+      <c r="O20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E050ECD3-7F4F-446C-9E00-FD6F9E1E4581}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="A3" sqref="A3:A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -694,7 +1222,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -711,7 +1239,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -728,7 +1256,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -745,7 +1273,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -762,24 +1290,24 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>150</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -796,9 +1324,9 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>980</v>
@@ -813,9 +1341,9 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>2.254</v>
@@ -830,7 +1358,7 @@
         <v>8.8559999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -847,7 +1375,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -864,9 +1392,9 @@
         <v>2.7864</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>1367</v>
@@ -881,9 +1409,9 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>3.1440999999999999</v>
@@ -898,9 +1426,9 @@
         <v>11.6424</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>104.5</v>
@@ -915,9 +1443,9 @@
         <v>106.9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>99.05</v>
@@ -932,9 +1460,9 @@
         <v>100.15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>93.6</v>
@@ -949,21 +1477,21 @@
         <v>93.4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -972,51 +1500,51 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC51449B-97CF-4FB9-B957-18B26D510E5F}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1033,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1050,7 +1578,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1067,7 +1595,7 @@
         <v>0.22700000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1084,7 +1612,7 @@
         <v>0.376</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1101,7 +1629,7 @@
         <v>0.42099999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1118,7 +1646,7 @@
         <v>0.45100000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1135,7 +1663,7 @@
         <v>0.46899999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1152,7 +1680,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1169,7 +1697,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1186,7 +1714,7 @@
         <v>0.40100000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1203,7 +1731,7 @@
         <v>0.33800000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1220,7 +1748,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1237,7 +1765,7 @@
         <v>0.21199999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1254,7 +1782,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1271,7 +1799,7 @@
         <v>0.13800000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1288,7 +1816,7 @@
         <v>0.114</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1305,7 +1833,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1322,7 +1850,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1339,7 +1867,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1356,7 +1884,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1373,7 +1901,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1390,7 +1918,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1407,7 +1935,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>24</v>
       </c>
@@ -1424,7 +1952,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1450,17 +1978,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414ADEED-6591-4152-9D56-99698B8D85E2}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1471,7 +1999,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1494,7 +2022,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -1517,7 +2045,7 @@
         <v>0.12504565517955238</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>250</v>
       </c>
@@ -1540,7 +2068,7 @@
         <v>0.11281836015960212</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>500</v>
       </c>
@@ -1563,7 +2091,7 @@
         <v>0.10059106513965184</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>750</v>
       </c>
@@ -1586,7 +2114,7 @@
         <v>8.836377011970159E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1000</v>
       </c>
@@ -1609,7 +2137,7 @@
         <v>7.6136475099751327E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1250</v>
       </c>
@@ -1632,7 +2160,7 @@
         <v>6.3909180079801065E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1500</v>
       </c>
@@ -1655,7 +2183,7 @@
         <v>5.1681885059850795E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1750</v>
       </c>
@@ -1678,7 +2206,7 @@
         <v>3.9454590039900525E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>2000</v>
       </c>
@@ -1701,7 +2229,7 @@
         <v>2.7227295019950262E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>2250</v>
       </c>
@@ -1724,7 +2252,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>2500</v>
       </c>
@@ -1747,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>2750</v>
       </c>
@@ -1770,7 +2298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>3000</v>
       </c>
@@ -1793,7 +2321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>3250</v>
       </c>
@@ -1816,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>3500</v>
       </c>
@@ -1839,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>3750</v>
       </c>
@@ -1862,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>4000</v>
       </c>
@@ -1885,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>4250</v>
       </c>
@@ -1908,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>4500</v>
       </c>
@@ -1931,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>4750</v>
       </c>
@@ -1954,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>5000</v>
       </c>
@@ -1977,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>5250</v>
       </c>
@@ -2000,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>5500</v>
       </c>
@@ -2023,7 +2551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>5750</v>
       </c>
@@ -2046,7 +2574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>6000</v>
       </c>
@@ -2075,7 +2603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D3E4DE-9E6C-44FE-BE28-2CC048DE88B1}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -2083,9 +2611,9 @@
       <selection activeCell="D3" sqref="D3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2096,7 +2624,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -2119,7 +2647,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>0</v>
       </c>
@@ -2142,7 +2670,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>250</v>
       </c>
@@ -2165,7 +2693,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>500</v>
       </c>
@@ -2188,7 +2716,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>750</v>
       </c>
@@ -2211,7 +2739,7 @@
         <v>7.9285714285714279E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>1000</v>
       </c>
@@ -2234,7 +2762,7 @@
         <v>6.8571428571428561E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>1250</v>
       </c>
@@ -2257,7 +2785,7 @@
         <v>5.7857142857142857E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>1500</v>
       </c>
@@ -2280,7 +2808,7 @@
         <v>4.7142857142857139E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>1750</v>
       </c>
@@ -2303,7 +2831,7 @@
         <v>3.6428571428571428E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>2000</v>
       </c>
@@ -2326,7 +2854,7 @@
         <v>2.5714285714285714E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>2250</v>
       </c>
@@ -2349,7 +2877,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>2500</v>
       </c>
@@ -2372,7 +2900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>2750</v>
       </c>
@@ -2395,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>3000</v>
       </c>
@@ -2418,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>3250</v>
       </c>
@@ -2441,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>3500</v>
       </c>
@@ -2464,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>3750</v>
       </c>
@@ -2487,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>4000</v>
       </c>
@@ -2510,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>4250</v>
       </c>
@@ -2533,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>4500</v>
       </c>
@@ -2556,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>4750</v>
       </c>
@@ -2579,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>5000</v>
       </c>
@@ -2602,7 +3130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>5250</v>
       </c>
@@ -2625,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>5500</v>
       </c>
@@ -2648,7 +3176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>5750</v>
       </c>
@@ -2671,7 +3199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>6000</v>
       </c>
@@ -2699,7 +3227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6402515-43FA-4DA9-864C-A5B5645E8FA7}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -2707,9 +3235,9 @@
       <selection activeCell="D3" sqref="D3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2720,7 +3248,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -2743,7 +3271,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -2766,7 +3294,7 @@
         <v>0.20020985915492956</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>250</v>
       </c>
@@ -2789,7 +3317,7 @@
         <v>0.19330075500221627</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>500</v>
       </c>
@@ -2812,7 +3340,7 @@
         <v>0.18208912433646085</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>750</v>
       </c>
@@ -2835,7 +3363,7 @@
         <v>0.17221962912793165</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>1000</v>
       </c>
@@ -2858,7 +3386,7 @@
         <v>0.16187026745572658</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>1250</v>
       </c>
@@ -2881,7 +3409,7 @@
         <v>0.15051436554863426</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1500</v>
       </c>
@@ -2904,7 +3432,7 @@
         <v>0.13982953181370789</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>1750</v>
       </c>
@@ -2927,7 +3455,7 @@
         <v>0.12963036004055509</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>2000</v>
       </c>
@@ -2950,7 +3478,7 @@
         <v>0.11979842221193718</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>2250</v>
       </c>
@@ -2973,7 +3501,7 @@
         <v>0.11025367270827484</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>2500</v>
       </c>
@@ -2996,7 +3524,7 @@
         <v>9.6251974695478831E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>2750</v>
       </c>
@@ -3019,7 +3547,7 @@
         <v>8.2356170875691664E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>3000</v>
       </c>
@@ -3042,7 +3570,7 @@
         <v>6.8859658865707024E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>3250</v>
       </c>
@@ -3065,7 +3593,7 @@
         <v>5.5701564370494352E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>3500</v>
       </c>
@@ -3088,7 +3616,7 @@
         <v>4.9309859154929581E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>3750</v>
       </c>
@@ -3111,7 +3639,7 @@
         <v>4.3309859154929582E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>4000</v>
       </c>
@@ -3134,7 +3662,7 @@
         <v>3.7309859154929577E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>4250</v>
       </c>
@@ -3157,7 +3685,7 @@
         <v>3.1309859154929578E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>4500</v>
       </c>
@@ -3180,7 +3708,7 @@
         <v>2.530985915492958E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>4750</v>
       </c>
@@ -3203,7 +3731,7 @@
         <v>1.9309859154929582E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>5000</v>
       </c>
@@ -3226,7 +3754,7 @@
         <v>1.3309859154929576E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>5250</v>
       </c>
@@ -3249,7 +3777,7 @@
         <v>7.3098591549295849E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>5500</v>
       </c>
@@ -3272,7 +3800,7 @@
         <v>1.3098591549295796E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>5750</v>
       </c>
@@ -3295,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>6000</v>
       </c>
@@ -3323,17 +3851,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E4A14F-CC8B-4DA2-B35F-37641B6E7671}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection sqref="A1:G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3344,7 +3872,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -3367,7 +3895,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -3390,7 +3918,7 @@
         <v>0.15539999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>250</v>
       </c>
@@ -3413,7 +3941,7 @@
         <v>0.1484908958472867</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>500</v>
       </c>
@@ -3436,7 +3964,7 @@
         <v>0.13727926518153127</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>750</v>
       </c>
@@ -3459,7 +3987,7 @@
         <v>0.12740976997300207</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>1000</v>
       </c>
@@ -3482,7 +4010,7 @@
         <v>0.117060408300797</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>1250</v>
       </c>
@@ -3505,7 +4033,7 @@
         <v>0.10570450639370468</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1500</v>
       </c>
@@ -3528,7 +4056,7 @@
         <v>9.5019672658778323E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>1750</v>
       </c>
@@ -3551,7 +4079,7 @@
         <v>8.482050088562551E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>2000</v>
       </c>
@@ -3574,7 +4102,7 @@
         <v>7.4988563057007615E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>2250</v>
       </c>
@@ -3597,7 +4125,7 @@
         <v>6.5443813553345262E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>2500</v>
       </c>
@@ -3620,7 +4148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>2750</v>
       </c>
@@ -3643,7 +4171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>3000</v>
       </c>
@@ -3666,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>3250</v>
       </c>
@@ -3689,7 +4217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>3500</v>
       </c>
@@ -3712,7 +4240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>3750</v>
       </c>
@@ -3735,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>4000</v>
       </c>
@@ -3758,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>4250</v>
       </c>
@@ -3781,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>4500</v>
       </c>
@@ -3804,7 +4332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>4750</v>
       </c>
@@ -3827,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>5000</v>
       </c>
@@ -3850,7 +4378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>5250</v>
       </c>
@@ -3873,7 +4401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>5500</v>
       </c>
@@ -3896,7 +4424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>5750</v>
       </c>
@@ -3919,7 +4447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>6000</v>
       </c>
@@ -3945,4 +4473,628 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F28858-6B58-488E-9ECB-52421D7FE941}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8">
+        <v>250</v>
+      </c>
+      <c r="C4" s="8">
+        <v>125</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>250</v>
+      </c>
+      <c r="B5" s="8">
+        <v>500</v>
+      </c>
+      <c r="C5" s="8">
+        <v>375</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>500</v>
+      </c>
+      <c r="B6" s="8">
+        <v>750</v>
+      </c>
+      <c r="C6" s="8">
+        <v>625</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>750</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="8">
+        <v>875</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1250</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1125</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>1250</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1500</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1375</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>1500</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1750</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1625</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>1750</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2000</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1875</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="8">
+        <v>2250</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2125</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>2250</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2500</v>
+      </c>
+      <c r="C13" s="8">
+        <v>2375</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>2500</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2750</v>
+      </c>
+      <c r="C14" s="8">
+        <v>2625</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>2750</v>
+      </c>
+      <c r="B15" s="8">
+        <v>3000</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2875</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>3000</v>
+      </c>
+      <c r="B16" s="8">
+        <v>3250</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3125</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>3250</v>
+      </c>
+      <c r="B17" s="8">
+        <v>3500</v>
+      </c>
+      <c r="C17" s="8">
+        <v>3375</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>3500</v>
+      </c>
+      <c r="B18" s="8">
+        <v>3750</v>
+      </c>
+      <c r="C18" s="8">
+        <v>3625</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>3750</v>
+      </c>
+      <c r="B19" s="8">
+        <v>4000</v>
+      </c>
+      <c r="C19" s="8">
+        <v>3875</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>4000</v>
+      </c>
+      <c r="B20" s="8">
+        <v>4250</v>
+      </c>
+      <c r="C20" s="8">
+        <v>4125</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>4250</v>
+      </c>
+      <c r="B21" s="8">
+        <v>4500</v>
+      </c>
+      <c r="C21" s="8">
+        <v>4375</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>4500</v>
+      </c>
+      <c r="B22" s="8">
+        <v>4750</v>
+      </c>
+      <c r="C22" s="8">
+        <v>4625</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>4750</v>
+      </c>
+      <c r="B23" s="8">
+        <v>5000</v>
+      </c>
+      <c r="C23" s="8">
+        <v>4875</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>5000</v>
+      </c>
+      <c r="B24" s="8">
+        <v>5250</v>
+      </c>
+      <c r="C24" s="8">
+        <v>5125</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>5250</v>
+      </c>
+      <c r="B25" s="8">
+        <v>5500</v>
+      </c>
+      <c r="C25" s="8">
+        <v>5375</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>5500</v>
+      </c>
+      <c r="B26" s="8">
+        <v>5750</v>
+      </c>
+      <c r="C26" s="8">
+        <v>5625</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>5750</v>
+      </c>
+      <c r="B27" s="8">
+        <v>6000</v>
+      </c>
+      <c r="C27" s="8">
+        <v>5875</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>6000</v>
+      </c>
+      <c r="B28" s="8">
+        <v>6250</v>
+      </c>
+      <c r="C28" s="8">
+        <v>6125</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>